<commit_message>
Adicion de users rules + correcciones
</commit_message>
<xml_diff>
--- a/Rules_Catalog.xlsx
+++ b/Rules_Catalog.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\DATA\PySpark\QR_4LL\Q-C_4LL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437F8C5-0364-46E8-A539-885F9F731C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8E8090-2469-4350-BB8E-F355407750DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quality Rules" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>quality_rule</t>
   </si>
@@ -37,49 +50,10 @@
     <t>rule_description</t>
   </si>
   <si>
-    <t>R_1_1</t>
-  </si>
-  <si>
     <t>Basics</t>
   </si>
   <si>
-    <t>Compara el data type esperado vs el data type real de la tabla</t>
-  </si>
-  <si>
-    <t>R_1_2</t>
-  </si>
-  <si>
-    <t>Chequea valores Nulos</t>
-  </si>
-  <si>
-    <t>R_1_3_D</t>
-  </si>
-  <si>
     <t>Valores específicos no permitidos. (Discretos)</t>
-  </si>
-  <si>
-    <t>R_1_3_C</t>
-  </si>
-  <si>
-    <t>Valores no permitidos (rangos)</t>
-  </si>
-  <si>
-    <t>R_1_4</t>
-  </si>
-  <si>
-    <t>Valores dentro del rango esperado</t>
-  </si>
-  <si>
-    <t>R_1_5</t>
-  </si>
-  <si>
-    <t>Valores dentro de un catálogo estático</t>
-  </si>
-  <si>
-    <t>R_1_6</t>
-  </si>
-  <si>
-    <t>Comprueba que no existan caracteres no deseados (whitespaces, otros caracteres)</t>
   </si>
   <si>
     <t>Chequea valores repetidos (duplicados, triplicados, etc.)</t>
@@ -88,10 +62,31 @@
     <t>Users</t>
   </si>
   <si>
-    <t>R_2_1</t>
+    <t>Controlar la relacion entre variables de tablas distintas.</t>
   </si>
   <si>
-    <t>R_2_2</t>
+    <t>Controlar la relacion entre variables de una misma tabla.</t>
+  </si>
+  <si>
+    <t>Controlar que la agregación de una variable no supere determinado umbral.</t>
+  </si>
+  <si>
+    <t>Comprueba que no existan caracteres no deseados.</t>
+  </si>
+  <si>
+    <t>Valores dentro de un catálogo estático.</t>
+  </si>
+  <si>
+    <t>Valores dentro del rango esperado.</t>
+  </si>
+  <si>
+    <t>Valores no permitidos (rangos).</t>
+  </si>
+  <si>
+    <t>Chequea valores Nulos.</t>
+  </si>
+  <si>
+    <t>Compara el data type esperado vs el data type real de la tabla.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +367,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -425,20 +420,21 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="str">
+        <f>"R_"&amp;B2&amp;"_"&amp;D2</f>
+        <v>R_1_1</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -465,20 +461,21 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
+      <c r="A3" s="4" t="str">
+        <f t="shared" ref="A3:A4" si="0">"R_"&amp;B3&amp;"_"&amp;D3</f>
+        <v>R_1_2</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -505,20 +502,21 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
+      <c r="A4" s="4" t="str">
+        <f>"R_"&amp;B4&amp;"_"&amp;D4&amp;"_D"</f>
+        <v>R_1_3_D</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -545,20 +543,21 @@
       <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
+      <c r="A5" s="4" t="str">
+        <f>"R_"&amp;B5&amp;"_"&amp;D5&amp;"_C"</f>
+        <v>R_1_3_C</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -585,20 +584,21 @@
       <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
+      <c r="A6" s="4" t="str">
+        <f>"R_"&amp;B6&amp;"_"&amp;D6</f>
+        <v>R_1_4</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -625,20 +625,21 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
+      <c r="A7" s="4" t="str">
+        <f t="shared" ref="A7:A8" si="1">"R_"&amp;B7&amp;"_"&amp;D7</f>
+        <v>R_1_5</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -665,20 +666,21 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
+      <c r="A8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>R_1_6</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -705,20 +707,21 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
+      <c r="A9" s="4" t="str">
+        <f>"R_"&amp;B9&amp;"_"&amp;D9</f>
+        <v>R_2_1</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -745,15 +748,22 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
+      <c r="A10" s="4" t="str">
+        <f>"R_"&amp;B10&amp;"_"&amp;D10</f>
+        <v>R_2_2</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -779,11 +789,22 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="4" t="str">
+        <f t="shared" ref="A11:A12" si="2">"R_"&amp;B11&amp;"_"&amp;D11</f>
+        <v>R_2_3</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -809,11 +830,22 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>R_2_4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>

</xml_diff>